<commit_message>
SKILIKS-3626. Add updated scenarios.
</commit_message>
<xml_diff>
--- a/media/scenario_tutorial_v23.0.xlsx
+++ b/media/scenario_tutorial_v23.0.xlsx
@@ -9559,6 +9559,87 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="22" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -9608,87 +9689,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -16176,7 +16176,7 @@
       <selection activeCell="F23" sqref="F23"/>
       <selection pane="topRight" activeCell="F23" sqref="F23"/>
       <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
-      <selection pane="bottomRight" activeCell="K3" sqref="K3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -16235,104 +16235,104 @@
   <sheetData>
     <row r="1" spans="1:84" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="V1" s="34"/>
-      <c r="W1" s="491" t="s">
+      <c r="W1" s="459" t="s">
         <v>575</v>
       </c>
-      <c r="X1" s="492"/>
-      <c r="Y1" s="493" t="s">
+      <c r="X1" s="460"/>
+      <c r="Y1" s="461" t="s">
         <v>576</v>
       </c>
-      <c r="Z1" s="494"/>
-      <c r="AA1" s="494"/>
-      <c r="AB1" s="494"/>
-      <c r="AC1" s="494"/>
-      <c r="AD1" s="494"/>
-      <c r="AE1" s="495"/>
-      <c r="AF1" s="496" t="s">
+      <c r="Z1" s="462"/>
+      <c r="AA1" s="462"/>
+      <c r="AB1" s="462"/>
+      <c r="AC1" s="462"/>
+      <c r="AD1" s="462"/>
+      <c r="AE1" s="463"/>
+      <c r="AF1" s="464" t="s">
         <v>577</v>
       </c>
-      <c r="AG1" s="497"/>
-      <c r="AH1" s="498" t="s">
+      <c r="AG1" s="465"/>
+      <c r="AH1" s="466" t="s">
         <v>578</v>
       </c>
-      <c r="AI1" s="499"/>
-      <c r="AJ1" s="500"/>
-      <c r="AK1" s="501" t="s">
+      <c r="AI1" s="467"/>
+      <c r="AJ1" s="468"/>
+      <c r="AK1" s="469" t="s">
         <v>579</v>
       </c>
-      <c r="AL1" s="502"/>
-      <c r="AM1" s="479" t="s">
+      <c r="AL1" s="470"/>
+      <c r="AM1" s="474" t="s">
         <v>580</v>
       </c>
-      <c r="AN1" s="480"/>
-      <c r="AO1" s="481"/>
-      <c r="AP1" s="482" t="s">
+      <c r="AN1" s="475"/>
+      <c r="AO1" s="476"/>
+      <c r="AP1" s="477" t="s">
         <v>581</v>
       </c>
-      <c r="AQ1" s="483"/>
-      <c r="AR1" s="484"/>
-      <c r="AS1" s="476" t="s">
+      <c r="AQ1" s="478"/>
+      <c r="AR1" s="479"/>
+      <c r="AS1" s="471" t="s">
         <v>582</v>
       </c>
-      <c r="AT1" s="477"/>
-      <c r="AU1" s="478"/>
-      <c r="AV1" s="485" t="s">
+      <c r="AT1" s="472"/>
+      <c r="AU1" s="473"/>
+      <c r="AV1" s="480" t="s">
         <v>583</v>
       </c>
-      <c r="AW1" s="486"/>
-      <c r="AX1" s="486"/>
-      <c r="AY1" s="486"/>
-      <c r="AZ1" s="486"/>
-      <c r="BA1" s="486"/>
-      <c r="BB1" s="487"/>
-      <c r="BC1" s="488" t="s">
+      <c r="AW1" s="481"/>
+      <c r="AX1" s="481"/>
+      <c r="AY1" s="481"/>
+      <c r="AZ1" s="481"/>
+      <c r="BA1" s="481"/>
+      <c r="BB1" s="482"/>
+      <c r="BC1" s="483" t="s">
         <v>584</v>
       </c>
-      <c r="BD1" s="489"/>
-      <c r="BE1" s="489"/>
-      <c r="BF1" s="490"/>
-      <c r="BG1" s="462" t="s">
+      <c r="BD1" s="484"/>
+      <c r="BE1" s="484"/>
+      <c r="BF1" s="485"/>
+      <c r="BG1" s="489" t="s">
         <v>585</v>
       </c>
-      <c r="BH1" s="463"/>
-      <c r="BI1" s="464"/>
+      <c r="BH1" s="490"/>
+      <c r="BI1" s="491"/>
       <c r="BJ1" s="389" t="s">
         <v>586</v>
       </c>
       <c r="BK1" s="390" t="s">
         <v>587</v>
       </c>
-      <c r="BL1" s="465" t="s">
+      <c r="BL1" s="492" t="s">
         <v>588</v>
       </c>
-      <c r="BM1" s="466"/>
-      <c r="BN1" s="467"/>
-      <c r="BO1" s="468" t="s">
+      <c r="BM1" s="493"/>
+      <c r="BN1" s="494"/>
+      <c r="BO1" s="495" t="s">
         <v>589</v>
       </c>
-      <c r="BP1" s="469"/>
+      <c r="BP1" s="496"/>
       <c r="BQ1" s="391" t="s">
         <v>590</v>
       </c>
-      <c r="BR1" s="470" t="s">
+      <c r="BR1" s="497" t="s">
         <v>591</v>
       </c>
-      <c r="BS1" s="471"/>
-      <c r="BT1" s="472"/>
-      <c r="BU1" s="473" t="s">
+      <c r="BS1" s="498"/>
+      <c r="BT1" s="499"/>
+      <c r="BU1" s="500" t="s">
         <v>592</v>
       </c>
-      <c r="BV1" s="474"/>
-      <c r="BW1" s="475"/>
+      <c r="BV1" s="501"/>
+      <c r="BW1" s="502"/>
       <c r="BX1" s="1"/>
       <c r="BY1" s="1"/>
       <c r="CB1" s="1"/>
-      <c r="CC1" s="459" t="s">
+      <c r="CC1" s="486" t="s">
         <v>657</v>
       </c>
-      <c r="CD1" s="460"/>
-      <c r="CE1" s="460"/>
-      <c r="CF1" s="461"/>
+      <c r="CD1" s="487"/>
+      <c r="CE1" s="487"/>
+      <c r="CF1" s="488"/>
     </row>
     <row r="2" spans="1:84" s="12" customFormat="1" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
@@ -17169,7 +17169,7 @@
         <v>565</v>
       </c>
       <c r="B7" s="305">
-        <v>41185</v>
+        <v>41550</v>
       </c>
       <c r="C7" s="207">
         <v>0.50347222222222221</v>
@@ -17455,7 +17455,7 @@
         <v>568</v>
       </c>
       <c r="B9" s="305">
-        <v>41185</v>
+        <v>41550</v>
       </c>
       <c r="C9" s="207">
         <v>0.42638888888888887</v>
@@ -17595,22 +17595,22 @@
   </sheetData>
   <autoFilter ref="A2:CF2"/>
   <mergeCells count="16">
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:AE1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AH1:AJ1"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AS1:AU1"/>
-    <mergeCell ref="AM1:AO1"/>
-    <mergeCell ref="AP1:AR1"/>
-    <mergeCell ref="AV1:BB1"/>
-    <mergeCell ref="BC1:BF1"/>
     <mergeCell ref="CC1:CF1"/>
     <mergeCell ref="BG1:BI1"/>
     <mergeCell ref="BL1:BN1"/>
     <mergeCell ref="BO1:BP1"/>
     <mergeCell ref="BR1:BT1"/>
     <mergeCell ref="BU1:BW1"/>
+    <mergeCell ref="AS1:AU1"/>
+    <mergeCell ref="AM1:AO1"/>
+    <mergeCell ref="AP1:AR1"/>
+    <mergeCell ref="AV1:BB1"/>
+    <mergeCell ref="BC1:BF1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AJ1"/>
+    <mergeCell ref="AK1:AL1"/>
   </mergeCells>
   <conditionalFormatting sqref="CF3">
     <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">

</xml_diff>